<commit_message>
Updated my walt disney
</commit_message>
<xml_diff>
--- a/challenge_4/Solution Sketch/Walt Disney - Raik.xlsx
+++ b/challenge_4/Solution Sketch/Walt Disney - Raik.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\BHH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raikolekannenberg/Desktop/GitHub/SmartSystemsBS14/challenge_4/Solution Sketch/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF095E9-180A-0547-A590-5B160BCB0AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Walt Disney Method</t>
   </si>
@@ -56,12 +57,30 @@
 • What is missing? 
 • What are weak points and how can we cope with them?</t>
   </si>
+  <si>
+    <t>Ferry´s that can alter the waterlevel, so that the ferry can allways operate. This generates more revenue which will be used for the captain´s salary and for the Ferry´s that need to be repared.</t>
+  </si>
+  <si>
+    <t>The ferry´s need to get upgraded so that they can alter the waterlevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there technologie for a Ferry that can alter the waterlevel? Is there enough revenue to pay the captains more money and repair the brooken ferry´s? </t>
+  </si>
+  <si>
+    <t>To implement the idea we need access to the diffrenet data to build the website. We need to caculate if selling beverages creates more revenue, so that the captains can be payed more.</t>
+  </si>
+  <si>
+    <t>Is there enough data to build a relaible website that the people can use. Is it possible to create enough revenue for the repairs and for the captains? Is crowed founding really realistic to pay for the repairs?</t>
+  </si>
+  <si>
+    <t>Build a better webpage that is more relaible, which uses data from diffrenent sources(watterlevel sensor, twitter api, hvv api….) and build a sign at the docks, which gives infos about the ferry´s (good for people who dont have access to the internet). Pay the captains more by getting more reveneu thro selling beverages on the docks and one the ferry´s. And use a crowed founding method to pay for the repairs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -122,6 +141,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Symbol"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,32 +191,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -396,21 +433,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="44.6328125" customWidth="1"/>
-    <col min="2" max="2" width="49.90625" customWidth="1"/>
-    <col min="3" max="3" width="65.7265625" customWidth="1"/>
+    <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.83203125" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
@@ -433,200 +470,212 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="65" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="49" customHeight="1">
+      <c r="A7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="89" customHeight="1">
+      <c r="A8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" ht="13">
+      <c r="A10" s="6"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" ht="12.5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" ht="12.5">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" ht="12.5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" ht="12.5">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" ht="12.5">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" ht="12.5">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" ht="12.5">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="12.5">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" ht="12.5">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" ht="12.5">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-    </row>
-    <row r="35" spans="1:3" ht="12.5">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="1:3" ht="12.5">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:3" ht="12.5">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" ht="12.5">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:3" ht="12.5">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-    </row>
-    <row r="40" spans="1:3" ht="12.5">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-    </row>
-    <row r="41" spans="1:3" ht="12.5">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="42" spans="1:3" ht="12.5">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" ht="13">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" ht="13">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3" ht="13">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" ht="13">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" ht="13">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" ht="13">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" ht="13">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" ht="13">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" ht="13">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" ht="13">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" ht="13">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" ht="13">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" ht="13">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" ht="13">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" ht="13">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" ht="13">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" ht="13">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" ht="13">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>